<commit_message>
Changes for replacing deprecated ExtentHTMLReporter for Extent Reporting
</commit_message>
<xml_diff>
--- a/src/dataEngine/invoicedemoFailScenario.xlsx
+++ b/src/dataEngine/invoicedemoFailScenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse-workspace\EngageReady\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FA9054-56C3-485A-9FA5-F65DA5ED0B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023BD584-C4C9-41F4-BAB3-73E8D2678666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B42BD951-151D-4FEC-98F1-EE6B5EDA39D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="311">
   <si>
     <t>Transaction_Name</t>
   </si>
@@ -5325,10 +5325,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F11B38-1DDE-49CC-8C51-2C4AA8C44AA2}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5340,7 +5340,7 @@
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="19" customFormat="1">
+    <row r="2" spans="1:10" s="19" customFormat="1">
       <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="19" customFormat="1">
+    <row r="3" spans="1:10" s="19" customFormat="1">
       <c r="A3" s="19" t="s">
         <v>16</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="19" customFormat="1">
+    <row r="4" spans="1:10" s="19" customFormat="1">
       <c r="A4" s="19" t="s">
         <v>176</v>
       </c>
@@ -5431,8 +5431,11 @@
       <c r="I4" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="19" customFormat="1">
+      <c r="J4" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="19" customFormat="1">
       <c r="A5" s="19" t="s">
         <v>176</v>
       </c>
@@ -5456,8 +5459,11 @@
       <c r="I5" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="19" customFormat="1">
+      <c r="J5" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="19" customFormat="1">
       <c r="A6" s="19" t="s">
         <v>176</v>
       </c>
@@ -5481,8 +5487,11 @@
       <c r="I6" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="19" customFormat="1">
+      <c r="J6" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="19" customFormat="1">
       <c r="A7" s="19" t="s">
         <v>176</v>
       </c>
@@ -5504,8 +5513,11 @@
       <c r="I7" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="19" customFormat="1">
+      <c r="J7" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="19" customFormat="1">
       <c r="A8" s="19" t="s">
         <v>176</v>
       </c>
@@ -5527,8 +5539,11 @@
       <c r="I8" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="19" customFormat="1">
+      <c r="J8" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="19" customFormat="1">
       <c r="A9" s="19" t="s">
         <v>176</v>
       </c>
@@ -5549,8 +5564,11 @@
       <c r="I9" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="19" customFormat="1">
+      <c r="J9" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="19" customFormat="1">
       <c r="A10" s="19" t="s">
         <v>176</v>
       </c>
@@ -5571,8 +5589,11 @@
       <c r="I10" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="19" customFormat="1">
+      <c r="J10" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="19" customFormat="1">
       <c r="A11" s="19" t="s">
         <v>176</v>
       </c>
@@ -5591,8 +5612,11 @@
       <c r="I11" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="19" customFormat="1">
+      <c r="J11" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="19" customFormat="1">
       <c r="A12" s="19" t="s">
         <v>176</v>
       </c>
@@ -5611,8 +5635,11 @@
       <c r="I12" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="19" customFormat="1">
+      <c r="J12" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="19" customFormat="1">
       <c r="A13" s="19" t="s">
         <v>176</v>
       </c>
@@ -5631,8 +5658,11 @@
       <c r="I13" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="19" customFormat="1">
+      <c r="J13" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="19" customFormat="1">
       <c r="B14" s="19" t="s">
         <v>66</v>
       </c>
@@ -5646,8 +5676,11 @@
       <c r="I14" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="19" customFormat="1">
+      <c r="J14" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="19" customFormat="1">
       <c r="A15" s="19" t="s">
         <v>176</v>
       </c>
@@ -5666,8 +5699,11 @@
       <c r="I15" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="19" customFormat="1">
+      <c r="J15" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="19" customFormat="1">
       <c r="A16" s="19" t="s">
         <v>176</v>
       </c>
@@ -5689,8 +5725,11 @@
       <c r="I16" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="19" customFormat="1">
+      <c r="J16" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="19" customFormat="1">
       <c r="A17" s="19" t="s">
         <v>176</v>
       </c>
@@ -5709,8 +5748,11 @@
       <c r="I17" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="19" customFormat="1">
+      <c r="J17" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="19" customFormat="1">
       <c r="A18" s="19" t="s">
         <v>176</v>
       </c>
@@ -5729,8 +5771,11 @@
       <c r="I18" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="19" customFormat="1">
+      <c r="J18" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="19" customFormat="1">
       <c r="A19" s="19" t="s">
         <v>176</v>
       </c>
@@ -5749,8 +5794,11 @@
       <c r="I19" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="19" customFormat="1">
+      <c r="J19" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="19" customFormat="1">
       <c r="A20" s="19" t="s">
         <v>176</v>
       </c>
@@ -5769,8 +5817,11 @@
       <c r="I20" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="19" customFormat="1">
+      <c r="J20" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="19" customFormat="1">
       <c r="A21" s="19" t="s">
         <v>176</v>
       </c>
@@ -5789,8 +5840,11 @@
       <c r="I21" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="19" customFormat="1">
+      <c r="J21" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="19" customFormat="1">
       <c r="B22" s="19" t="s">
         <v>86</v>
       </c>
@@ -5806,8 +5860,11 @@
       <c r="I22" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" s="19" customFormat="1">
+      <c r="J22" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="19" customFormat="1">
       <c r="B23" s="19" t="s">
         <v>87</v>
       </c>
@@ -5823,8 +5880,11 @@
       <c r="I23" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" s="19" customFormat="1">
+      <c r="J23" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="19" customFormat="1">
       <c r="B24" s="19" t="s">
         <v>89</v>
       </c>
@@ -5840,8 +5900,11 @@
       <c r="I24" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1">
+      <c r="J24" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="19" customFormat="1">
       <c r="B25" s="19" t="s">
         <v>92</v>
       </c>
@@ -5857,8 +5920,11 @@
       <c r="I25" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="19" t="s">
         <v>37</v>
       </c>
@@ -5880,8 +5946,11 @@
       <c r="I26" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="19" t="s">
         <v>37</v>
       </c>
@@ -5903,8 +5972,11 @@
       <c r="I27" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="19" t="s">
         <v>37</v>
       </c>
@@ -5926,8 +5998,11 @@
       <c r="I28" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="19" t="s">
         <v>37</v>
       </c>
@@ -5949,8 +6024,11 @@
       <c r="I29" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="19"/>
       <c r="B30" s="19" t="s">
         <v>104</v>
@@ -5968,8 +6046,11 @@
       <c r="I30" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="19"/>
       <c r="B31" s="19" t="s">
         <v>105</v>
@@ -5987,8 +6068,11 @@
       <c r="I31" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="19"/>
       <c r="B32" s="19" t="s">
         <v>108</v>
@@ -6006,8 +6090,11 @@
       <c r="I32" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="19"/>
       <c r="B33" s="19" t="s">
         <v>109</v>
@@ -6025,8 +6112,11 @@
       <c r="I33" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="19"/>
       <c r="B34" s="19" t="s">
         <v>111</v>
@@ -6044,8 +6134,11 @@
       <c r="I34" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="19"/>
       <c r="B35" s="19" t="s">
         <v>112</v>
@@ -6063,8 +6156,11 @@
       <c r="I35" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="19" t="s">
         <v>37</v>
       </c>
@@ -6086,8 +6182,11 @@
       <c r="I36" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="19" t="s">
         <v>37</v>
       </c>
@@ -6109,8 +6208,11 @@
       <c r="I37" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="19" t="s">
         <v>37</v>
       </c>
@@ -6132,8 +6234,11 @@
       <c r="I38" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="19" t="s">
         <v>37</v>
       </c>
@@ -6155,8 +6260,11 @@
       <c r="I39" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="19" t="s">
         <v>37</v>
       </c>
@@ -6178,8 +6286,11 @@
       <c r="I40" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="19" t="s">
         <v>37</v>
       </c>
@@ -6201,8 +6312,11 @@
       <c r="I41" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="19" t="s">
         <v>37</v>
       </c>
@@ -6224,8 +6338,11 @@
       <c r="I42" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
@@ -6247,8 +6364,11 @@
       <c r="I43" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="19" t="s">
         <v>37</v>
       </c>
@@ -6270,8 +6390,11 @@
       <c r="I44" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="19" t="s">
         <v>37</v>
       </c>
@@ -6291,8 +6414,11 @@
       <c r="I45" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="19" t="s">
         <v>37</v>
       </c>
@@ -6312,8 +6438,11 @@
       <c r="I46" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="19" t="s">
         <v>37</v>
       </c>
@@ -6333,8 +6462,11 @@
       <c r="I47" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="19" t="s">
         <v>37</v>
       </c>
@@ -6356,8 +6488,11 @@
       <c r="I48" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="19" t="s">
         <v>37</v>
       </c>
@@ -6379,8 +6514,11 @@
       <c r="I49" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="19" t="s">
         <v>37</v>
       </c>
@@ -6400,8 +6538,11 @@
       <c r="I50" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="19" t="s">
         <v>37</v>
       </c>
@@ -6421,8 +6562,11 @@
       <c r="I51" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="19" t="s">
         <v>37</v>
       </c>
@@ -6442,8 +6586,11 @@
       <c r="I52" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="19" t="s">
         <v>37</v>
       </c>
@@ -6461,8 +6608,11 @@
       <c r="I53" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="19" t="s">
         <v>37</v>
       </c>
@@ -6482,8 +6632,11 @@
       <c r="I54" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="19" t="s">
         <v>37</v>
       </c>
@@ -6503,8 +6656,11 @@
       <c r="I55" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="19" t="s">
         <v>37</v>
       </c>
@@ -6524,8 +6680,11 @@
       <c r="I56" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="19" t="s">
         <v>37</v>
       </c>
@@ -6545,8 +6704,11 @@
       <c r="I57" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="19" t="s">
         <v>37</v>
       </c>
@@ -6566,8 +6728,11 @@
       <c r="I58" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="19" t="s">
         <v>37</v>
       </c>
@@ -6585,6 +6750,9 @@
       <c r="G59" s="19"/>
       <c r="H59" s="19"/>
       <c r="I59" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" s="19" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made changes to pull out helper actions from DriverScript
</commit_message>
<xml_diff>
--- a/src/dataEngine/invoicedemoFailScenario.xlsx
+++ b/src/dataEngine/invoicedemoFailScenario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse-workspace\EngageReady\src\dataEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gjoshi2\Documents\EclipseWorkspace\Gitlab\EngageReady\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023BD584-C4C9-41F4-BAB3-73E8D2678666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18775B8D-42EB-4E2F-B2BB-DA2B9B30AEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B42BD951-151D-4FEC-98F1-EE6B5EDA39D0}"/>
   </bookViews>
@@ -31,12 +31,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="312">
   <si>
     <t>Transaction_Name</t>
   </si>
@@ -969,6 +977,9 @@
   </si>
   <si>
     <t>INV-0000231</t>
+  </si>
+  <si>
+    <t>openBrowserWithoutSecurity</t>
   </si>
 </sst>
 </file>
@@ -5327,8 +5338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F11B38-1DDE-49CC-8C51-2C4AA8C44AA2}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5380,7 +5391,7 @@
         <v>200</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>201</v>
+        <v>311</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>295</v>

</xml_diff>